<commit_message>
refining report algorithm for sqlalchemy data source
</commit_message>
<xml_diff>
--- a/error_data.xlsx
+++ b/error_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21690" windowHeight="9195"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21690" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
   <si>
     <t>phone_number:4435679068</t>
   </si>
@@ -653,7 +653,7 @@
   <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,9 +730,8 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>call_id:"1496982"</v>
+      <c r="C6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>